<commit_message>
O sistema cria assim o excel. Adicionei uma 'conta paga' como exemplo.
</commit_message>
<xml_diff>
--- a/Conta.xlsx
+++ b/Conta.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,29 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Claro</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12/06/2023</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Um exemplo!
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>